<commit_message>
RBA v2.4 - Alteração da pasta de origem
</commit_message>
<xml_diff>
--- a/ArquivosGerados/RelatorioBuscaAtiva.xlsx
+++ b/ArquivosGerados/RelatorioBuscaAtiva.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="180">
   <si>
     <t>Risco Reprova por Falta</t>
   </si>
@@ -88,24 +88,24 @@
     <t>Daniele Farias De Souza</t>
   </si>
   <si>
+    <t>Maria Rafaela Lopes De Oliveira</t>
+  </si>
+  <si>
     <t>Gabrielly Oliveira Costa</t>
   </si>
   <si>
     <t>Nicolas Ribeiro Domiciano Dos Santos</t>
   </si>
   <si>
-    <t>Maria Rafaela Lopes De Oliveira</t>
-  </si>
-  <si>
     <t>Joao Vitor De Freitas Lucas</t>
   </si>
   <si>
+    <t>Ana Sarah Dos Santos Barbosa</t>
+  </si>
+  <si>
     <t>Kimberly Soares De Araujo</t>
   </si>
   <si>
-    <t>Ana Sarah Dos Santos Barbosa</t>
-  </si>
-  <si>
     <t>Nicolas Gutierres Silva</t>
   </si>
   <si>
@@ -124,27 +124,174 @@
     <t>Giulianna Vilas Boas Luque</t>
   </si>
   <si>
+    <t>Pedro Henrique Ferreira Fontao</t>
+  </si>
+  <si>
     <t>Debora Gomes Palmeira</t>
   </si>
   <si>
-    <t>Pedro Henrique Ferreira Fontao</t>
-  </si>
-  <si>
     <t>Carlos Eduardo Siqueira Alves</t>
   </si>
   <si>
+    <t>Ryan Carvalho Cirqueira Mendes</t>
+  </si>
+  <si>
     <t>Nara Ashelley Almeida Pacheco</t>
   </si>
   <si>
-    <t>Ryan Carvalho Cirqueira Mendes</t>
-  </si>
-  <si>
     <t>Alexia Da Silva Santana</t>
   </si>
   <si>
     <t>Igor Da Silva Marques</t>
   </si>
   <si>
+    <t>William Lippert Dos Santos</t>
+  </si>
+  <si>
+    <t>Gustavo Santos Silva</t>
+  </si>
+  <si>
+    <t>Isaac Mendes Ferreira</t>
+  </si>
+  <si>
+    <t>Isabella Sousa De Jesus</t>
+  </si>
+  <si>
+    <t>Felipe Felix Rodrigues</t>
+  </si>
+  <si>
+    <t>Jamile Vitoria De Oliveira Campos</t>
+  </si>
+  <si>
+    <t>Eduardo Souza Rodrigues</t>
+  </si>
+  <si>
+    <t>Kaique Henrique Costa Santos</t>
+  </si>
+  <si>
+    <t>Lais Bispo De Jesus</t>
+  </si>
+  <si>
+    <t>Julio Cezar Silva Da Costa</t>
+  </si>
+  <si>
+    <t>Vitor Braga Lima</t>
+  </si>
+  <si>
+    <t>Cleyton Lima Aguiar</t>
+  </si>
+  <si>
+    <t>Kaiky Nascimento Izidio</t>
+  </si>
+  <si>
+    <t>Airton Gabriel De Oliveira Gomes</t>
+  </si>
+  <si>
+    <t>Juan Da Silva Santos</t>
+  </si>
+  <si>
+    <t>Leonardo Lopes Marques</t>
+  </si>
+  <si>
+    <t>Matheus Alves Timota</t>
+  </si>
+  <si>
+    <t>Kauã Gonsalves De Souza</t>
+  </si>
+  <si>
+    <t>Giovanna Lima Delmiro</t>
+  </si>
+  <si>
+    <t>Amanda Rodrigues Silva</t>
+  </si>
+  <si>
+    <t>Grazielle De Sousa Santos</t>
+  </si>
+  <si>
+    <t>Jhemenson Sampaio Matos</t>
+  </si>
+  <si>
+    <t>Pedro Henrique Braga Silva</t>
+  </si>
+  <si>
+    <t>Kauanny Dutra Faustino</t>
+  </si>
+  <si>
+    <t>Cássia Hellen Aguiar De Souza</t>
+  </si>
+  <si>
+    <t>Mireia Ferreira De Sousa</t>
+  </si>
+  <si>
+    <t>Nicolly De Oliveira Da Costa</t>
+  </si>
+  <si>
+    <t>Manuela De Paula Santos De Araujo</t>
+  </si>
+  <si>
+    <t>Thamara Melissa Lins Da Silva</t>
+  </si>
+  <si>
+    <t>Ana Beatriz Teixeira Da Silva</t>
+  </si>
+  <si>
+    <t>Rafael Sales Do Nascimento</t>
+  </si>
+  <si>
+    <t>Gabriel Batista De Souza</t>
+  </si>
+  <si>
+    <t>Arthur Davi Xavier Lima</t>
+  </si>
+  <si>
+    <t>Luis Carlos Da Silva</t>
+  </si>
+  <si>
+    <t>Joao Pedro Pereira Dos Santos</t>
+  </si>
+  <si>
+    <t>Adryan Garcia Medeiros</t>
+  </si>
+  <si>
+    <t>Jamilton Dos Santos Macêdo</t>
+  </si>
+  <si>
+    <t>Thallys Miranda Ribeiro</t>
+  </si>
+  <si>
+    <t>Pedro Jesus Dos Santos</t>
+  </si>
+  <si>
+    <t>Kayla Soares Silva</t>
+  </si>
+  <si>
+    <t>Richard Silva Dos Santos</t>
+  </si>
+  <si>
+    <t>Maria Eduarda Farias De Araujo</t>
+  </si>
+  <si>
+    <t>Felipe Borges De Sousa</t>
+  </si>
+  <si>
+    <t>Antonio Italo Gomes Da Costa</t>
+  </si>
+  <si>
+    <t>Jamily Medeiros Herculano</t>
+  </si>
+  <si>
+    <t>Pedro Lucca Ribeiro Balbo</t>
+  </si>
+  <si>
+    <t>Maria Fernanda Oliveira Da Silva</t>
+  </si>
+  <si>
+    <t>Rayssa Monica De Lima Santos</t>
+  </si>
+  <si>
+    <t>Renan Moreira Da Cruz</t>
+  </si>
+  <si>
     <t>Ativo</t>
   </si>
   <si>
@@ -178,24 +325,24 @@
     <t>000112544246 - 3</t>
   </si>
   <si>
+    <t>000111767502 - 6</t>
+  </si>
+  <si>
     <t>000111746428 - 3</t>
   </si>
   <si>
     <t>000112901736 - 9</t>
   </si>
   <si>
-    <t>000111767502 - 6</t>
-  </si>
-  <si>
     <t>000111756985 - 8</t>
   </si>
   <si>
+    <t>000111888078 - X</t>
+  </si>
+  <si>
     <t>000112683774 - X</t>
   </si>
   <si>
-    <t>000111888078 - X</t>
-  </si>
-  <si>
     <t>000112547318 - 6</t>
   </si>
   <si>
@@ -214,27 +361,162 @@
     <t>000110364901 - 2</t>
   </si>
   <si>
+    <t>000115042364 - X</t>
+  </si>
+  <si>
     <t>000112169740 - 9</t>
   </si>
   <si>
-    <t>000115042364 - X</t>
-  </si>
-  <si>
     <t>000110363365 - X</t>
   </si>
   <si>
+    <t>000110318713 - 2</t>
+  </si>
+  <si>
     <t>000110084186 - 6</t>
   </si>
   <si>
-    <t>000110318713 - 2</t>
-  </si>
-  <si>
     <t>000111327535 - 2</t>
   </si>
   <si>
     <t>000114905590 - X</t>
   </si>
   <si>
+    <t>000111322331 - 5</t>
+  </si>
+  <si>
+    <t>000110317865 - 9</t>
+  </si>
+  <si>
+    <t>000111305148 - 6</t>
+  </si>
+  <si>
+    <t>000109371400 - 1</t>
+  </si>
+  <si>
+    <t>000110387786 - 0</t>
+  </si>
+  <si>
+    <t>000109454582 - X</t>
+  </si>
+  <si>
+    <t>000111327533 - 9</t>
+  </si>
+  <si>
+    <t>000111812977 - 5</t>
+  </si>
+  <si>
+    <t>000111767601 - 8</t>
+  </si>
+  <si>
+    <t>000109342848 - X</t>
+  </si>
+  <si>
+    <t>000109312615 - 2</t>
+  </si>
+  <si>
+    <t>000111813019 - 4</t>
+  </si>
+  <si>
+    <t>000110446539 - 5</t>
+  </si>
+  <si>
+    <t>000111305153 - X</t>
+  </si>
+  <si>
+    <t>000111304764 - 1</t>
+  </si>
+  <si>
+    <t>000109454498 - X</t>
+  </si>
+  <si>
+    <t>000112320997 - 2</t>
+  </si>
+  <si>
+    <t>000111687133 - 6</t>
+  </si>
+  <si>
+    <t>000109335423 - 9</t>
+  </si>
+  <si>
+    <t>000108418046 - 7</t>
+  </si>
+  <si>
+    <t>000110315260 - 9</t>
+  </si>
+  <si>
+    <t>000122595955 - X</t>
+  </si>
+  <si>
+    <t>000111103532 - 5</t>
+  </si>
+  <si>
+    <t>000107302012 - 5</t>
+  </si>
+  <si>
+    <t>000123349569 - 0</t>
+  </si>
+  <si>
+    <t>000121552441 - 9</t>
+  </si>
+  <si>
+    <t>000109454443 - 7</t>
+  </si>
+  <si>
+    <t>000111327662 - 9</t>
+  </si>
+  <si>
+    <t>000109968828 - 0</t>
+  </si>
+  <si>
+    <t>000109454486 - 3</t>
+  </si>
+  <si>
+    <t>000114575408 - 9</t>
+  </si>
+  <si>
+    <t>000113408321 - X</t>
+  </si>
+  <si>
+    <t>000113704722 - 7</t>
+  </si>
+  <si>
+    <t>000114070941 - 0</t>
+  </si>
+  <si>
+    <t>000115896857 - 7</t>
+  </si>
+  <si>
+    <t>000116717267 - X</t>
+  </si>
+  <si>
+    <t>000115652507 - X</t>
+  </si>
+  <si>
+    <t>000114643929 - 5</t>
+  </si>
+  <si>
+    <t>000114714421 - 7</t>
+  </si>
+  <si>
+    <t>000114555263 - 8</t>
+  </si>
+  <si>
+    <t>000112845699 - 0</t>
+  </si>
+  <si>
+    <t>000112473637 - 2</t>
+  </si>
+  <si>
+    <t>000113284754 - 0</t>
+  </si>
+  <si>
+    <t>000114501585 - 2</t>
+  </si>
+  <si>
+    <t>000113793459 - 1</t>
+  </si>
+  <si>
     <t>1ª SERIE A INTEGRAL ANUAL</t>
   </si>
   <si>
@@ -242,6 +524,36 @@
   </si>
   <si>
     <t>1ª SERIE C INTEGRAL ANUAL</t>
+  </si>
+  <si>
+    <t>2ª SERIE A INTEGRAL ANUAL</t>
+  </si>
+  <si>
+    <t>2ª SERIE B INTEGRAL ANUAL</t>
+  </si>
+  <si>
+    <t>2ª SERIE C INTEGRAL ANUAL</t>
+  </si>
+  <si>
+    <t>3ª SERIE A INTEGRAL ANUAL</t>
+  </si>
+  <si>
+    <t>3ª SERIE B INTEGRAL ANUAL</t>
+  </si>
+  <si>
+    <t>3ª SERIE C INTEGRAL ANUAL</t>
+  </si>
+  <si>
+    <t>6° ANO A INTEGRAL ANUAL</t>
+  </si>
+  <si>
+    <t>6° ANO B INTEGRAL ANUAL</t>
+  </si>
+  <si>
+    <t>6° ANO C INTEGRAL ANUAL</t>
+  </si>
+  <si>
+    <t>6° ANO D INTEGRAL ANUAL</t>
   </si>
 </sst>
 </file>
@@ -603,7 +915,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -667,13 +979,13 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F2">
         <v>0.6</v>
       </c>
       <c r="G2">
-        <v>0.38</v>
+        <v>0.37</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -691,10 +1003,10 @@
         <v>900090102973</v>
       </c>
       <c r="M2" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="N2" t="s">
-        <v>73</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -711,13 +1023,13 @@
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F3">
         <v>0.61</v>
       </c>
       <c r="G3">
-        <v>0.71</v>
+        <v>0.63</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -735,10 +1047,10 @@
         <v>900104786820</v>
       </c>
       <c r="M3" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="N3" t="s">
-        <v>73</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -755,13 +1067,13 @@
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F4">
         <v>0.65</v>
       </c>
       <c r="G4">
-        <v>0.38</v>
+        <v>0.37</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -779,10 +1091,10 @@
         <v>900090226507</v>
       </c>
       <c r="M4" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="N4" t="s">
-        <v>73</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -799,13 +1111,13 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F5">
         <v>0.66</v>
       </c>
       <c r="G5">
-        <v>0.79</v>
+        <v>0.74</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -823,10 +1135,10 @@
         <v>900105963198</v>
       </c>
       <c r="M5" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="N5" t="s">
-        <v>73</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -843,13 +1155,13 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F6">
         <v>0.6899999999999999</v>
       </c>
       <c r="G6">
-        <v>0.54</v>
+        <v>0.58</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -867,10 +1179,10 @@
         <v>900090147805</v>
       </c>
       <c r="M6" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="N6" t="s">
-        <v>73</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -887,13 +1199,13 @@
         <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F7">
         <v>0.6899999999999999</v>
       </c>
       <c r="G7">
-        <v>0.67</v>
+        <v>0.68</v>
       </c>
       <c r="H7">
         <v>0.25</v>
@@ -911,10 +1223,10 @@
         <v>900090246311</v>
       </c>
       <c r="M7" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="N7" t="s">
-        <v>73</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -931,13 +1243,13 @@
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F8">
         <v>0.71</v>
       </c>
       <c r="G8">
-        <v>0.46</v>
+        <v>0.32</v>
       </c>
       <c r="H8">
         <v>0.38</v>
@@ -955,10 +1267,10 @@
         <v>900090331260</v>
       </c>
       <c r="M8" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="N8" t="s">
-        <v>73</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -975,13 +1287,13 @@
         <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F9">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
       <c r="G9">
-        <v>0.88</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <v>0.13</v>
@@ -999,10 +1311,10 @@
         <v>900111109369</v>
       </c>
       <c r="M9" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="N9" t="s">
-        <v>73</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -1019,13 +1331,13 @@
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F10">
-        <v>0.53</v>
+        <v>0.52</v>
       </c>
       <c r="G10">
-        <v>0.79</v>
+        <v>0.72</v>
       </c>
       <c r="H10">
         <v>0.05</v>
@@ -1043,10 +1355,10 @@
         <v>900105621655</v>
       </c>
       <c r="M10" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="N10" t="s">
-        <v>74</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -1063,10 +1375,10 @@
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F11">
-        <v>0.62</v>
+        <v>0.6</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1087,10 +1399,10 @@
         <v>900108711161</v>
       </c>
       <c r="M11" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="N11" t="s">
-        <v>74</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1098,7 +1410,7 @@
         <v>1</v>
       </c>
       <c r="B12">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
@@ -1107,34 +1419,34 @@
         <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F12">
-        <v>0.6899999999999999</v>
+        <v>0.68</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>0.72</v>
       </c>
       <c r="H12">
-        <v>0.14</v>
+        <v>0.29</v>
       </c>
       <c r="I12" s="2">
-        <v>44960</v>
+        <v>45156</v>
       </c>
       <c r="J12" s="2">
         <v>45275</v>
       </c>
       <c r="K12">
-        <v>29217645</v>
+        <v>29238719</v>
       </c>
       <c r="L12">
-        <v>900090089520</v>
+        <v>900108574436</v>
       </c>
       <c r="M12" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="N12" t="s">
-        <v>74</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1142,43 +1454,43 @@
         <v>1</v>
       </c>
       <c r="B13">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
       </c>
       <c r="D13">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F13">
-        <v>0.7</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="G13">
-        <v>0.9399999999999999</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>0.05</v>
+        <v>0.14</v>
       </c>
       <c r="I13" s="2">
-        <v>44963</v>
+        <v>44960</v>
       </c>
       <c r="J13" s="2">
         <v>45275</v>
       </c>
       <c r="K13">
-        <v>30372950</v>
+        <v>29217645</v>
       </c>
       <c r="L13">
-        <v>900100936307</v>
+        <v>900090089520</v>
       </c>
       <c r="M13" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="N13" t="s">
-        <v>74</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1186,43 +1498,43 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
       </c>
       <c r="D14">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F14">
-        <v>0.7</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="G14">
-        <v>0.79</v>
+        <v>0.92</v>
       </c>
       <c r="H14">
-        <v>0.29</v>
+        <v>0.05</v>
       </c>
       <c r="I14" s="2">
-        <v>45156</v>
+        <v>44963</v>
       </c>
       <c r="J14" s="2">
         <v>45275</v>
       </c>
       <c r="K14">
-        <v>29238719</v>
+        <v>30372950</v>
       </c>
       <c r="L14">
-        <v>900108574436</v>
+        <v>900100936307</v>
       </c>
       <c r="M14" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="N14" t="s">
-        <v>74</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -1239,13 +1551,13 @@
         <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F15">
         <v>0.71</v>
       </c>
       <c r="G15">
-        <v>0.62</v>
+        <v>0.72</v>
       </c>
       <c r="H15">
         <v>0.05</v>
@@ -1263,10 +1575,10 @@
         <v>900090228923</v>
       </c>
       <c r="M15" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="N15" t="s">
-        <v>74</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -1274,25 +1586,25 @@
         <v>1</v>
       </c>
       <c r="B16">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
         <v>28</v>
       </c>
       <c r="D16">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F16">
         <v>0.72</v>
       </c>
       <c r="G16">
-        <v>0.82</v>
+        <v>0.76</v>
       </c>
       <c r="H16">
-        <v>0.05</v>
+        <v>0.14</v>
       </c>
       <c r="I16" s="2">
         <v>44960</v>
@@ -1301,16 +1613,16 @@
         <v>45275</v>
       </c>
       <c r="K16">
-        <v>30154988</v>
+        <v>29359295</v>
       </c>
       <c r="L16">
-        <v>900090207807</v>
+        <v>900090276927</v>
       </c>
       <c r="M16" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="N16" t="s">
-        <v>74</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -1318,25 +1630,25 @@
         <v>1</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
         <v>29</v>
       </c>
       <c r="D17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F17">
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
       <c r="G17">
-        <v>0.82</v>
+        <v>1</v>
       </c>
       <c r="H17">
-        <v>0.14</v>
+        <v>0.05</v>
       </c>
       <c r="I17" s="2">
         <v>44960</v>
@@ -1345,16 +1657,16 @@
         <v>45275</v>
       </c>
       <c r="K17">
-        <v>29359295</v>
+        <v>30154988</v>
       </c>
       <c r="L17">
-        <v>900090276927</v>
+        <v>900090207807</v>
       </c>
       <c r="M17" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="N17" t="s">
-        <v>74</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -1371,13 +1683,13 @@
         <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F18">
         <v>0.73</v>
       </c>
       <c r="G18">
-        <v>0.82</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <v>0.05</v>
@@ -1395,10 +1707,10 @@
         <v>900090103734</v>
       </c>
       <c r="M18" t="s">
-        <v>60</v>
+        <v>109</v>
       </c>
       <c r="N18" t="s">
-        <v>74</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -1415,16 +1727,16 @@
         <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F19">
-        <v>0.48</v>
+        <v>0.47</v>
       </c>
       <c r="G19">
-        <v>0.17</v>
+        <v>0.1</v>
       </c>
       <c r="H19">
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="I19" s="2">
         <v>45026</v>
@@ -1439,10 +1751,10 @@
         <v>900104854117</v>
       </c>
       <c r="M19" t="s">
-        <v>61</v>
+        <v>110</v>
       </c>
       <c r="N19" t="s">
-        <v>75</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -1459,16 +1771,16 @@
         <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F20">
         <v>0.6</v>
       </c>
       <c r="G20">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="H20">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I20" s="2">
         <v>44967</v>
@@ -1483,10 +1795,10 @@
         <v>900101484358</v>
       </c>
       <c r="M20" t="s">
-        <v>62</v>
+        <v>111</v>
       </c>
       <c r="N20" t="s">
-        <v>75</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1503,16 +1815,16 @@
         <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F21">
         <v>0.6</v>
       </c>
       <c r="G21">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="H21">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I21" s="2">
         <v>44972</v>
@@ -1527,10 +1839,10 @@
         <v>900101795279</v>
       </c>
       <c r="M21" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="N21" t="s">
-        <v>75</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1547,16 +1859,16 @@
         <v>15</v>
       </c>
       <c r="E22" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F22">
-        <v>0.65</v>
+        <v>0.63</v>
       </c>
       <c r="G22">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H22">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I22" s="2">
         <v>45057</v>
@@ -1571,10 +1883,10 @@
         <v>900105604998</v>
       </c>
       <c r="M22" t="s">
-        <v>64</v>
+        <v>113</v>
       </c>
       <c r="N22" t="s">
-        <v>75</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -1591,16 +1903,16 @@
         <v>16</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F23">
         <v>0.66</v>
       </c>
       <c r="G23">
-        <v>0.63</v>
+        <v>0.8</v>
       </c>
       <c r="H23">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I23" s="2">
         <v>45000</v>
@@ -1615,10 +1927,10 @@
         <v>900103910690</v>
       </c>
       <c r="M23" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
       <c r="N23" t="s">
-        <v>75</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1626,7 +1938,7 @@
         <v>1</v>
       </c>
       <c r="B24">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
         <v>36</v>
@@ -1635,34 +1947,34 @@
         <v>16</v>
       </c>
       <c r="E24" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F24">
-        <v>0.6899999999999999</v>
+        <v>0.68</v>
       </c>
       <c r="G24">
-        <v>0.67</v>
+        <v>0.6</v>
       </c>
       <c r="H24">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I24" s="2">
-        <v>44991</v>
+        <v>44960</v>
       </c>
       <c r="J24" s="2">
         <v>45275</v>
       </c>
       <c r="K24">
-        <v>29640956</v>
+        <v>32508533</v>
       </c>
       <c r="L24">
-        <v>900103223814</v>
+        <v>900090239981</v>
       </c>
       <c r="M24" t="s">
-        <v>66</v>
+        <v>115</v>
       </c>
       <c r="N24" t="s">
-        <v>75</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -1670,7 +1982,7 @@
         <v>1</v>
       </c>
       <c r="B25">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="C25" t="s">
         <v>37</v>
@@ -1679,34 +1991,34 @@
         <v>16</v>
       </c>
       <c r="E25" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F25">
         <v>0.6899999999999999</v>
       </c>
       <c r="G25">
-        <v>0.73</v>
+        <v>0.85</v>
       </c>
       <c r="H25">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I25" s="2">
-        <v>44960</v>
+        <v>44991</v>
       </c>
       <c r="J25" s="2">
         <v>45275</v>
       </c>
       <c r="K25">
-        <v>32508533</v>
+        <v>29640956</v>
       </c>
       <c r="L25">
-        <v>900090239981</v>
+        <v>900103223814</v>
       </c>
       <c r="M25" t="s">
-        <v>67</v>
+        <v>116</v>
       </c>
       <c r="N25" t="s">
-        <v>75</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -1723,16 +2035,16 @@
         <v>16</v>
       </c>
       <c r="E26" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F26">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="G26">
         <v>0.7</v>
       </c>
-      <c r="G26">
-        <v>0.8</v>
-      </c>
       <c r="H26">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I26" s="2">
         <v>45029</v>
@@ -1747,10 +2059,10 @@
         <v>900104967293</v>
       </c>
       <c r="M26" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="N26" t="s">
-        <v>75</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -1758,43 +2070,43 @@
         <v>1</v>
       </c>
       <c r="B27">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
         <v>39</v>
       </c>
       <c r="D27">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E27" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F27">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
       <c r="G27">
-        <v>0.83</v>
+        <v>1</v>
       </c>
       <c r="H27">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I27" s="2">
-        <v>45194</v>
+        <v>45051</v>
       </c>
       <c r="J27" s="2">
         <v>45275</v>
       </c>
       <c r="K27">
-        <v>27555405</v>
+        <v>27789932</v>
       </c>
       <c r="L27">
-        <v>900111115992</v>
+        <v>900105484322</v>
       </c>
       <c r="M27" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="N27" t="s">
-        <v>75</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -1802,43 +2114,43 @@
         <v>1</v>
       </c>
       <c r="B28">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
         <v>40</v>
       </c>
       <c r="D28">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E28" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F28">
-        <v>0.72</v>
+        <v>0.71</v>
       </c>
       <c r="G28">
-        <v>0.83</v>
+        <v>1</v>
       </c>
       <c r="H28">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I28" s="2">
-        <v>45051</v>
+        <v>45194</v>
       </c>
       <c r="J28" s="2">
         <v>45275</v>
       </c>
       <c r="K28">
-        <v>27789932</v>
+        <v>27555405</v>
       </c>
       <c r="L28">
-        <v>900105484322</v>
+        <v>900111115992</v>
       </c>
       <c r="M28" t="s">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="N28" t="s">
-        <v>75</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -1855,16 +2167,16 @@
         <v>18</v>
       </c>
       <c r="E29" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F29">
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
       <c r="G29">
-        <v>0.77</v>
+        <v>0.7</v>
       </c>
       <c r="H29">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I29" s="2">
         <v>44960</v>
@@ -1879,10 +2191,10 @@
         <v>900100500500</v>
       </c>
       <c r="M29" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="N29" t="s">
-        <v>75</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -1899,16 +2211,16 @@
         <v>15</v>
       </c>
       <c r="E30" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F30">
-        <v>0.74</v>
+        <v>0.73</v>
       </c>
       <c r="G30">
         <v>1</v>
       </c>
       <c r="H30">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I30" s="2">
         <v>44960</v>
@@ -1923,10 +2235,2154 @@
         <v>900090491973</v>
       </c>
       <c r="M30" t="s">
+        <v>121</v>
+      </c>
+      <c r="N30" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>33</v>
+      </c>
+      <c r="C31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31">
+        <v>17</v>
+      </c>
+      <c r="E31" t="s">
+        <v>92</v>
+      </c>
+      <c r="F31">
+        <v>0.63</v>
+      </c>
+      <c r="G31">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2">
+        <v>44963</v>
+      </c>
+      <c r="J31" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K31">
+        <v>28793548</v>
+      </c>
+      <c r="L31">
+        <v>900100937264</v>
+      </c>
+      <c r="M31" t="s">
+        <v>122</v>
+      </c>
+      <c r="N31" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32">
+        <v>18</v>
+      </c>
+      <c r="E32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32">
+        <v>0.65</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J32" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K32">
+        <v>27789084</v>
+      </c>
+      <c r="L32">
+        <v>900100290910</v>
+      </c>
+      <c r="M32" t="s">
+        <v>123</v>
+      </c>
+      <c r="N32" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33">
+        <v>17</v>
+      </c>
+      <c r="E33" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33">
+        <v>0.72</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J33" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K33">
+        <v>28776365</v>
+      </c>
+      <c r="L33">
+        <v>900095472326</v>
+      </c>
+      <c r="M33" t="s">
+        <v>124</v>
+      </c>
+      <c r="N33" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34">
+        <v>16</v>
+      </c>
+      <c r="E34" t="s">
+        <v>92</v>
+      </c>
+      <c r="F34">
+        <v>0.72</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34" s="2">
+        <v>45061</v>
+      </c>
+      <c r="J34" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K34">
+        <v>26842619</v>
+      </c>
+      <c r="L34">
+        <v>900105658610</v>
+      </c>
+      <c r="M34" t="s">
+        <v>125</v>
+      </c>
+      <c r="N34" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35">
+        <v>16</v>
+      </c>
+      <c r="E35" t="s">
+        <v>92</v>
+      </c>
+      <c r="F35">
+        <v>0.75</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>0.73</v>
+      </c>
+      <c r="I35" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J35" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K35">
+        <v>27859005</v>
+      </c>
+      <c r="L35">
+        <v>900095472298</v>
+      </c>
+      <c r="M35" t="s">
+        <v>126</v>
+      </c>
+      <c r="N35" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>16</v>
+      </c>
+      <c r="C36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36">
+        <v>17</v>
+      </c>
+      <c r="E36" t="s">
+        <v>92</v>
+      </c>
+      <c r="F36">
+        <v>0.55</v>
+      </c>
+      <c r="G36">
+        <v>0.47</v>
+      </c>
+      <c r="H36">
+        <v>0.13</v>
+      </c>
+      <c r="I36" s="2">
+        <v>44991</v>
+      </c>
+      <c r="J36" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K36">
+        <v>26925801</v>
+      </c>
+      <c r="L36">
+        <v>900103176746</v>
+      </c>
+      <c r="M36" t="s">
+        <v>127</v>
+      </c>
+      <c r="N36" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>43</v>
+      </c>
+      <c r="C37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37">
+        <v>18</v>
+      </c>
+      <c r="E37" t="s">
+        <v>92</v>
+      </c>
+      <c r="F37">
+        <v>0.62</v>
+      </c>
+      <c r="G37">
+        <v>0.89</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37" s="2">
+        <v>45197</v>
+      </c>
+      <c r="J37" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K37">
+        <v>28798750</v>
+      </c>
+      <c r="L37">
+        <v>900111354891</v>
+      </c>
+      <c r="M37" t="s">
+        <v>128</v>
+      </c>
+      <c r="N37" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>19</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38">
+        <v>17</v>
+      </c>
+      <c r="E38" t="s">
+        <v>92</v>
+      </c>
+      <c r="F38">
+        <v>0.64</v>
+      </c>
+      <c r="G38">
+        <v>0.74</v>
+      </c>
+      <c r="H38">
+        <v>0.67</v>
+      </c>
+      <c r="I38" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J38" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K38">
+        <v>29284194</v>
+      </c>
+      <c r="L38">
+        <v>900095472786</v>
+      </c>
+      <c r="M38" t="s">
+        <v>129</v>
+      </c>
+      <c r="N38" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>37</v>
+      </c>
+      <c r="C39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39">
+        <v>16</v>
+      </c>
+      <c r="E39" t="s">
+        <v>92</v>
+      </c>
+      <c r="F39">
+        <v>0.64</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>0.13</v>
+      </c>
+      <c r="I39" s="2">
+        <v>45013</v>
+      </c>
+      <c r="J39" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K39">
+        <v>29238818</v>
+      </c>
+      <c r="L39">
+        <v>900104495021</v>
+      </c>
+      <c r="M39" t="s">
+        <v>130</v>
+      </c>
+      <c r="N39" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>41</v>
+      </c>
+      <c r="C40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40">
+        <v>16</v>
+      </c>
+      <c r="E40" t="s">
+        <v>92</v>
+      </c>
+      <c r="F40">
+        <v>0.65</v>
+      </c>
+      <c r="G40">
+        <v>0.42</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40" s="2">
+        <v>45054</v>
+      </c>
+      <c r="J40" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K40">
+        <v>26814067</v>
+      </c>
+      <c r="L40">
+        <v>900105515854</v>
+      </c>
+      <c r="M40" t="s">
+        <v>131</v>
+      </c>
+      <c r="N40" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>36</v>
+      </c>
+      <c r="C41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41">
+        <v>17</v>
+      </c>
+      <c r="E41" t="s">
+        <v>92</v>
+      </c>
+      <c r="F41">
+        <v>0.7</v>
+      </c>
+      <c r="G41">
+        <v>0.58</v>
+      </c>
+      <c r="H41">
+        <v>0.13</v>
+      </c>
+      <c r="I41" s="2">
+        <v>44999</v>
+      </c>
+      <c r="J41" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K41">
+        <v>26783834</v>
+      </c>
+      <c r="L41">
+        <v>900103820474</v>
+      </c>
+      <c r="M41" t="s">
+        <v>132</v>
+      </c>
+      <c r="N41" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>42</v>
+      </c>
+      <c r="C42" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42">
+        <v>16</v>
+      </c>
+      <c r="E42" t="s">
+        <v>92</v>
+      </c>
+      <c r="F42">
+        <v>0.72</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>0.13</v>
+      </c>
+      <c r="I42" s="2">
+        <v>45147</v>
+      </c>
+      <c r="J42" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K42">
+        <v>29284236</v>
+      </c>
+      <c r="L42">
+        <v>900108406011</v>
+      </c>
+      <c r="M42" t="s">
+        <v>133</v>
+      </c>
+      <c r="N42" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>18</v>
+      </c>
+      <c r="C43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43">
+        <v>16</v>
+      </c>
+      <c r="E43" t="s">
+        <v>92</v>
+      </c>
+      <c r="F43">
+        <v>0.74</v>
+      </c>
+      <c r="G43">
+        <v>0.47</v>
+      </c>
+      <c r="H43">
+        <v>0.27</v>
+      </c>
+      <c r="I43" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J43" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K43">
+        <v>27917758</v>
+      </c>
+      <c r="L43">
+        <v>900086950075</v>
+      </c>
+      <c r="M43" t="s">
+        <v>134</v>
+      </c>
+      <c r="N43" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>38</v>
+      </c>
+      <c r="C44" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44">
+        <v>16</v>
+      </c>
+      <c r="E44" t="s">
+        <v>92</v>
+      </c>
+      <c r="F44">
+        <v>0.36</v>
+      </c>
+      <c r="G44">
+        <v>0.11</v>
+      </c>
+      <c r="H44">
+        <v>0.25</v>
+      </c>
+      <c r="I44" s="2">
+        <v>45147</v>
+      </c>
+      <c r="J44" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K44">
+        <v>28776370</v>
+      </c>
+      <c r="L44">
+        <v>900108406032</v>
+      </c>
+      <c r="M44" t="s">
+        <v>135</v>
+      </c>
+      <c r="N44" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>36</v>
+      </c>
+      <c r="C45" t="s">
+        <v>57</v>
+      </c>
+      <c r="D45">
+        <v>16</v>
+      </c>
+      <c r="E45" t="s">
+        <v>92</v>
+      </c>
+      <c r="F45">
+        <v>0.57</v>
+      </c>
+      <c r="G45">
+        <v>0.89</v>
+      </c>
+      <c r="H45">
+        <v>0.25</v>
+      </c>
+      <c r="I45" s="2">
+        <v>45070</v>
+      </c>
+      <c r="J45" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K45">
+        <v>28775981</v>
+      </c>
+      <c r="L45">
+        <v>900105833922</v>
+      </c>
+      <c r="M45" t="s">
+        <v>136</v>
+      </c>
+      <c r="N45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>23</v>
+      </c>
+      <c r="C46" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46">
+        <v>17</v>
+      </c>
+      <c r="E46" t="s">
+        <v>92</v>
+      </c>
+      <c r="F46">
+        <v>0.74</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>0.25</v>
+      </c>
+      <c r="I46" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J46" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K46">
+        <v>26925717</v>
+      </c>
+      <c r="L46">
+        <v>900094700131</v>
+      </c>
+      <c r="M46" t="s">
+        <v>137</v>
+      </c>
+      <c r="N46" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>27</v>
+      </c>
+      <c r="C47" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47">
+        <v>17</v>
+      </c>
+      <c r="E47" t="s">
+        <v>92</v>
+      </c>
+      <c r="F47">
+        <v>0.75</v>
+      </c>
+      <c r="G47">
+        <v>0.79</v>
+      </c>
+      <c r="H47">
+        <v>0.25</v>
+      </c>
+      <c r="I47" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J47" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K47">
+        <v>29792213</v>
+      </c>
+      <c r="L47">
+        <v>900094699995</v>
+      </c>
+      <c r="M47" t="s">
+        <v>138</v>
+      </c>
+      <c r="N47" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48">
+        <v>33</v>
+      </c>
+      <c r="C48" t="s">
+        <v>60</v>
+      </c>
+      <c r="D48">
+        <v>17</v>
+      </c>
+      <c r="E48" t="s">
+        <v>92</v>
+      </c>
+      <c r="F48">
+        <v>0.58</v>
+      </c>
+      <c r="G48">
+        <v>0.82</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48" s="2">
+        <v>45183</v>
+      </c>
+      <c r="J48" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K48">
+        <v>29158350</v>
+      </c>
+      <c r="L48">
+        <v>900108870873</v>
+      </c>
+      <c r="M48" t="s">
+        <v>139</v>
+      </c>
+      <c r="N48" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49">
+        <v>18</v>
+      </c>
+      <c r="E49" t="s">
+        <v>92</v>
+      </c>
+      <c r="F49">
+        <v>0.62</v>
+      </c>
+      <c r="G49">
+        <v>0.82</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J49" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K49">
+        <v>26806642</v>
+      </c>
+      <c r="L49">
+        <v>900086945388</v>
+      </c>
+      <c r="M49" t="s">
+        <v>140</v>
+      </c>
+      <c r="N49" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>31</v>
+      </c>
+      <c r="C50" t="s">
+        <v>62</v>
+      </c>
+      <c r="D50">
+        <v>18</v>
+      </c>
+      <c r="E50" t="s">
+        <v>92</v>
+      </c>
+      <c r="F50">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="G50">
+        <v>0.55</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50" s="2">
+        <v>44999</v>
+      </c>
+      <c r="J50" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K50">
+        <v>25889266</v>
+      </c>
+      <c r="L50">
+        <v>900103820355</v>
+      </c>
+      <c r="M50" t="s">
+        <v>141</v>
+      </c>
+      <c r="N50" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51">
+        <v>19</v>
+      </c>
+      <c r="E51" t="s">
+        <v>92</v>
+      </c>
+      <c r="F51">
+        <v>0.72</v>
+      </c>
+      <c r="G51">
+        <v>0.82</v>
+      </c>
+      <c r="H51">
+        <v>0.29</v>
+      </c>
+      <c r="I51" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J51" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K51">
+        <v>27786479</v>
+      </c>
+      <c r="L51">
+        <v>900086945363</v>
+      </c>
+      <c r="M51" t="s">
+        <v>142</v>
+      </c>
+      <c r="N51" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>10</v>
+      </c>
+      <c r="C52" t="s">
+        <v>64</v>
+      </c>
+      <c r="D52">
+        <v>18</v>
+      </c>
+      <c r="E52" t="s">
+        <v>92</v>
+      </c>
+      <c r="F52">
+        <v>0.72</v>
+      </c>
+      <c r="G52">
+        <v>0.82</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J52" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K52">
+        <v>37596017</v>
+      </c>
+      <c r="L52">
+        <v>900086945392</v>
+      </c>
+      <c r="M52" t="s">
+        <v>143</v>
+      </c>
+      <c r="N52" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>20</v>
+      </c>
+      <c r="C53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D53">
+        <v>18</v>
+      </c>
+      <c r="E53" t="s">
+        <v>92</v>
+      </c>
+      <c r="F53">
+        <v>0.59</v>
+      </c>
+      <c r="G53">
+        <v>0.33</v>
+      </c>
+      <c r="H53">
+        <v>0.5</v>
+      </c>
+      <c r="I53" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J53" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K53">
+        <v>28574749</v>
+      </c>
+      <c r="L53">
+        <v>900086946162</v>
+      </c>
+      <c r="M53" t="s">
+        <v>144</v>
+      </c>
+      <c r="N53" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>12</v>
+      </c>
+      <c r="C54" t="s">
+        <v>66</v>
+      </c>
+      <c r="D54">
+        <v>17</v>
+      </c>
+      <c r="E54" t="s">
+        <v>92</v>
+      </c>
+      <c r="F54">
+        <v>0.61</v>
+      </c>
+      <c r="G54">
+        <v>0.67</v>
+      </c>
+      <c r="H54">
+        <v>0.5</v>
+      </c>
+      <c r="I54" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J54" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K54">
+        <v>24773235</v>
+      </c>
+      <c r="L54">
+        <v>900086946157</v>
+      </c>
+      <c r="M54" t="s">
+        <v>145</v>
+      </c>
+      <c r="N54" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55" t="s">
+        <v>67</v>
+      </c>
+      <c r="D55">
+        <v>18</v>
+      </c>
+      <c r="E55" t="s">
+        <v>92</v>
+      </c>
+      <c r="F55">
+        <v>0.64</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>0.5</v>
+      </c>
+      <c r="I55" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J55" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K55">
+        <v>38349614</v>
+      </c>
+      <c r="L55">
+        <v>900086946178</v>
+      </c>
+      <c r="M55" t="s">
+        <v>146</v>
+      </c>
+      <c r="N55" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56">
+        <v>33</v>
+      </c>
+      <c r="C56" t="s">
+        <v>68</v>
+      </c>
+      <c r="D56">
+        <v>17</v>
+      </c>
+      <c r="E56" t="s">
+        <v>92</v>
+      </c>
+      <c r="F56">
+        <v>0.64</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>0.5</v>
+      </c>
+      <c r="I56" s="2">
+        <v>45013</v>
+      </c>
+      <c r="J56" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K56">
+        <v>36552483</v>
+      </c>
+      <c r="L56">
+        <v>900104513089</v>
+      </c>
+      <c r="M56" t="s">
+        <v>147</v>
+      </c>
+      <c r="N56" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>18</v>
+      </c>
+      <c r="C57" t="s">
+        <v>69</v>
+      </c>
+      <c r="D57">
+        <v>18</v>
+      </c>
+      <c r="E57" t="s">
+        <v>92</v>
+      </c>
+      <c r="F57">
+        <v>0.66</v>
+      </c>
+      <c r="G57">
+        <v>0.33</v>
+      </c>
+      <c r="H57">
+        <v>0.5</v>
+      </c>
+      <c r="I57" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J57" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K57">
+        <v>26925662</v>
+      </c>
+      <c r="L57">
+        <v>900086946147</v>
+      </c>
+      <c r="M57" t="s">
+        <v>148</v>
+      </c>
+      <c r="N57" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <v>15</v>
+      </c>
+      <c r="C58" t="s">
+        <v>70</v>
+      </c>
+      <c r="D58">
+        <v>18</v>
+      </c>
+      <c r="E58" t="s">
+        <v>92</v>
+      </c>
+      <c r="F58">
+        <v>0.7</v>
+      </c>
+      <c r="G58">
+        <v>0.67</v>
+      </c>
+      <c r="H58">
+        <v>0.5</v>
+      </c>
+      <c r="I58" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J58" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K58">
+        <v>28798879</v>
+      </c>
+      <c r="L58">
+        <v>900086946161</v>
+      </c>
+      <c r="M58" t="s">
+        <v>149</v>
+      </c>
+      <c r="N58" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>26</v>
+      </c>
+      <c r="C59" t="s">
+        <v>71</v>
+      </c>
+      <c r="D59">
+        <v>17</v>
+      </c>
+      <c r="E59" t="s">
+        <v>92</v>
+      </c>
+      <c r="F59">
+        <v>0.7</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>0.5</v>
+      </c>
+      <c r="I59" s="2">
+        <v>44992</v>
+      </c>
+      <c r="J59" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K59">
+        <v>27440047</v>
+      </c>
+      <c r="L59">
+        <v>900103320179</v>
+      </c>
+      <c r="M59" t="s">
+        <v>150</v>
+      </c>
+      <c r="N59" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
         <v>72</v>
       </c>
-      <c r="N30" t="s">
+      <c r="D60">
+        <v>17</v>
+      </c>
+      <c r="E60" t="s">
+        <v>92</v>
+      </c>
+      <c r="F60">
+        <v>0.71</v>
+      </c>
+      <c r="G60">
+        <v>0.67</v>
+      </c>
+      <c r="H60">
+        <v>0.5</v>
+      </c>
+      <c r="I60" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J60" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K60">
+        <v>26925705</v>
+      </c>
+      <c r="L60">
+        <v>900086946141</v>
+      </c>
+      <c r="M60" t="s">
+        <v>151</v>
+      </c>
+      <c r="N60" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>21</v>
+      </c>
+      <c r="C61" t="s">
+        <v>73</v>
+      </c>
+      <c r="D61">
+        <v>18</v>
+      </c>
+      <c r="E61" t="s">
+        <v>92</v>
+      </c>
+      <c r="F61">
+        <v>0.32</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0.44</v>
+      </c>
+      <c r="I61" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J61" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K61">
+        <v>28908078</v>
+      </c>
+      <c r="L61">
+        <v>900086947411</v>
+      </c>
+      <c r="N61" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>35</v>
+      </c>
+      <c r="C62" t="s">
+        <v>74</v>
+      </c>
+      <c r="D62">
+        <v>11</v>
+      </c>
+      <c r="E62" t="s">
+        <v>92</v>
+      </c>
+      <c r="F62">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0.05</v>
+      </c>
+      <c r="I62" s="2">
+        <v>45161</v>
+      </c>
+      <c r="J62" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K62">
+        <v>31549604</v>
+      </c>
+      <c r="L62">
+        <v>900108631688</v>
+      </c>
+      <c r="N62" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>36</v>
+      </c>
+      <c r="C63" t="s">
         <v>75</v>
+      </c>
+      <c r="D63">
+        <v>11</v>
+      </c>
+      <c r="E63" t="s">
+        <v>92</v>
+      </c>
+      <c r="F63">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="G63">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63" s="2">
+        <v>45216</v>
+      </c>
+      <c r="J63" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K63">
+        <v>32041580</v>
+      </c>
+      <c r="L63">
+        <v>900114081252</v>
+      </c>
+      <c r="M63" t="s">
+        <v>152</v>
+      </c>
+      <c r="N63" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>31</v>
+      </c>
+      <c r="C64" t="s">
+        <v>76</v>
+      </c>
+      <c r="D64">
+        <v>11</v>
+      </c>
+      <c r="E64" t="s">
+        <v>92</v>
+      </c>
+      <c r="F64">
+        <v>0.6</v>
+      </c>
+      <c r="G64">
+        <v>0.96</v>
+      </c>
+      <c r="H64">
+        <v>0.95</v>
+      </c>
+      <c r="I64" s="2">
+        <v>45035</v>
+      </c>
+      <c r="J64" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K64">
+        <v>30879534</v>
+      </c>
+      <c r="L64">
+        <v>900105112348</v>
+      </c>
+      <c r="M64" t="s">
+        <v>153</v>
+      </c>
+      <c r="N64" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65">
+        <v>13</v>
+      </c>
+      <c r="C65" t="s">
+        <v>77</v>
+      </c>
+      <c r="D65">
+        <v>11</v>
+      </c>
+      <c r="E65" t="s">
+        <v>92</v>
+      </c>
+      <c r="F65">
+        <v>0.62</v>
+      </c>
+      <c r="G65">
+        <v>0.79</v>
+      </c>
+      <c r="H65">
+        <v>0.43</v>
+      </c>
+      <c r="I65" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J65" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K65">
+        <v>31175935</v>
+      </c>
+      <c r="L65">
+        <v>900090163444</v>
+      </c>
+      <c r="M65" t="s">
+        <v>154</v>
+      </c>
+      <c r="N65" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>78</v>
+      </c>
+      <c r="D66">
+        <v>12</v>
+      </c>
+      <c r="E66" t="s">
+        <v>92</v>
+      </c>
+      <c r="F66">
+        <v>0.63</v>
+      </c>
+      <c r="G66">
+        <v>0.71</v>
+      </c>
+      <c r="H66">
+        <v>0.57</v>
+      </c>
+      <c r="I66" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J66" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K66">
+        <v>31537707</v>
+      </c>
+      <c r="L66">
+        <v>900090068553</v>
+      </c>
+      <c r="M66" t="s">
+        <v>155</v>
+      </c>
+      <c r="N66" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14">
+      <c r="A67">
+        <v>1</v>
+      </c>
+      <c r="B67">
+        <v>43</v>
+      </c>
+      <c r="C67" t="s">
+        <v>79</v>
+      </c>
+      <c r="D67">
+        <v>14</v>
+      </c>
+      <c r="E67" t="s">
+        <v>92</v>
+      </c>
+      <c r="F67">
+        <v>0.34</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0.14</v>
+      </c>
+      <c r="I67" s="2">
+        <v>45050</v>
+      </c>
+      <c r="J67" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K67">
+        <v>39560623</v>
+      </c>
+      <c r="L67">
+        <v>900105444758</v>
+      </c>
+      <c r="N67" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14">
+      <c r="A68">
+        <v>1</v>
+      </c>
+      <c r="B68">
+        <v>52</v>
+      </c>
+      <c r="C68" t="s">
+        <v>80</v>
+      </c>
+      <c r="D68">
+        <v>12</v>
+      </c>
+      <c r="E68" t="s">
+        <v>92</v>
+      </c>
+      <c r="F68">
+        <v>0.38</v>
+      </c>
+      <c r="G68">
+        <v>0.46</v>
+      </c>
+      <c r="H68">
+        <v>0.38</v>
+      </c>
+      <c r="I68" s="2">
+        <v>45156</v>
+      </c>
+      <c r="J68" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K68">
+        <v>33363026</v>
+      </c>
+      <c r="L68">
+        <v>900108570964</v>
+      </c>
+      <c r="M68" t="s">
+        <v>156</v>
+      </c>
+      <c r="N68" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14">
+      <c r="A69">
+        <v>1</v>
+      </c>
+      <c r="B69">
+        <v>50</v>
+      </c>
+      <c r="C69" t="s">
+        <v>81</v>
+      </c>
+      <c r="D69">
+        <v>12</v>
+      </c>
+      <c r="E69" t="s">
+        <v>92</v>
+      </c>
+      <c r="F69">
+        <v>0.7</v>
+      </c>
+      <c r="G69">
+        <v>0.93</v>
+      </c>
+      <c r="H69">
+        <v>0.52</v>
+      </c>
+      <c r="I69" s="2">
+        <v>45141</v>
+      </c>
+      <c r="J69" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K69">
+        <v>34183436</v>
+      </c>
+      <c r="L69">
+        <v>900108293662</v>
+      </c>
+      <c r="M69" t="s">
+        <v>157</v>
+      </c>
+      <c r="N69" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14">
+      <c r="A70">
+        <v>1</v>
+      </c>
+      <c r="B70">
+        <v>49</v>
+      </c>
+      <c r="C70" t="s">
+        <v>82</v>
+      </c>
+      <c r="D70">
+        <v>12</v>
+      </c>
+      <c r="E70" t="s">
+        <v>92</v>
+      </c>
+      <c r="F70">
+        <v>0.73</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="I70" s="2">
+        <v>45141</v>
+      </c>
+      <c r="J70" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K70">
+        <v>33118676</v>
+      </c>
+      <c r="L70">
+        <v>900108290490</v>
+      </c>
+      <c r="M70" t="s">
+        <v>158</v>
+      </c>
+      <c r="N70" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14">
+      <c r="A71">
+        <v>1</v>
+      </c>
+      <c r="B71">
+        <v>34</v>
+      </c>
+      <c r="C71" t="s">
+        <v>83</v>
+      </c>
+      <c r="D71">
+        <v>11</v>
+      </c>
+      <c r="E71" t="s">
+        <v>92</v>
+      </c>
+      <c r="F71">
+        <v>0.4</v>
+      </c>
+      <c r="G71">
+        <v>0.5</v>
+      </c>
+      <c r="H71">
+        <v>0.24</v>
+      </c>
+      <c r="I71" s="2">
+        <v>45084</v>
+      </c>
+      <c r="J71" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K71">
+        <v>32110101</v>
+      </c>
+      <c r="L71">
+        <v>900106062997</v>
+      </c>
+      <c r="M71" t="s">
+        <v>159</v>
+      </c>
+      <c r="N71" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14">
+      <c r="A72">
+        <v>1</v>
+      </c>
+      <c r="B72">
+        <v>32</v>
+      </c>
+      <c r="C72" t="s">
+        <v>84</v>
+      </c>
+      <c r="D72">
+        <v>12</v>
+      </c>
+      <c r="E72" t="s">
+        <v>92</v>
+      </c>
+      <c r="F72">
+        <v>0.44</v>
+      </c>
+      <c r="G72">
+        <v>0.36</v>
+      </c>
+      <c r="H72">
+        <v>0.38</v>
+      </c>
+      <c r="I72" s="2">
+        <v>45001</v>
+      </c>
+      <c r="J72" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K72">
+        <v>32258266</v>
+      </c>
+      <c r="L72">
+        <v>900103970616</v>
+      </c>
+      <c r="N72" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14">
+      <c r="A73">
+        <v>1</v>
+      </c>
+      <c r="B73">
+        <v>9</v>
+      </c>
+      <c r="C73" t="s">
+        <v>85</v>
+      </c>
+      <c r="D73">
+        <v>11</v>
+      </c>
+      <c r="E73" t="s">
+        <v>92</v>
+      </c>
+      <c r="F73">
+        <v>0.64</v>
+      </c>
+      <c r="G73">
+        <v>0.21</v>
+      </c>
+      <c r="H73">
+        <v>0.48</v>
+      </c>
+      <c r="I73" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J73" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K73">
+        <v>32180593</v>
+      </c>
+      <c r="L73">
+        <v>900099548474</v>
+      </c>
+      <c r="M73" t="s">
+        <v>160</v>
+      </c>
+      <c r="N73" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14">
+      <c r="A74">
+        <v>1</v>
+      </c>
+      <c r="B74">
+        <v>3</v>
+      </c>
+      <c r="C74" t="s">
+        <v>86</v>
+      </c>
+      <c r="D74">
+        <v>11</v>
+      </c>
+      <c r="E74" t="s">
+        <v>92</v>
+      </c>
+      <c r="F74">
+        <v>0.66</v>
+      </c>
+      <c r="G74">
+        <v>0.79</v>
+      </c>
+      <c r="H74">
+        <v>0.43</v>
+      </c>
+      <c r="I74" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J74" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K74">
+        <v>32021435</v>
+      </c>
+      <c r="L74">
+        <v>900091952933</v>
+      </c>
+      <c r="M74" t="s">
+        <v>161</v>
+      </c>
+      <c r="N74" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14">
+      <c r="A75">
+        <v>1</v>
+      </c>
+      <c r="B75">
+        <v>35</v>
+      </c>
+      <c r="C75" t="s">
+        <v>87</v>
+      </c>
+      <c r="D75">
+        <v>12</v>
+      </c>
+      <c r="E75" t="s">
+        <v>92</v>
+      </c>
+      <c r="F75">
+        <v>0.33</v>
+      </c>
+      <c r="G75">
+        <v>0.29</v>
+      </c>
+      <c r="H75">
+        <v>0.24</v>
+      </c>
+      <c r="I75" s="2">
+        <v>45163</v>
+      </c>
+      <c r="J75" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K75">
+        <v>30316913</v>
+      </c>
+      <c r="L75">
+        <v>900108661427</v>
+      </c>
+      <c r="M75" t="s">
+        <v>162</v>
+      </c>
+      <c r="N75" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14">
+      <c r="A76">
+        <v>1</v>
+      </c>
+      <c r="B76">
+        <v>26</v>
+      </c>
+      <c r="C76" t="s">
+        <v>88</v>
+      </c>
+      <c r="D76">
+        <v>14</v>
+      </c>
+      <c r="E76" t="s">
+        <v>92</v>
+      </c>
+      <c r="F76">
+        <v>0.6</v>
+      </c>
+      <c r="G76">
+        <v>0.5</v>
+      </c>
+      <c r="H76">
+        <v>0.29</v>
+      </c>
+      <c r="I76" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J76" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K76">
+        <v>29944852</v>
+      </c>
+      <c r="L76">
+        <v>900095872343</v>
+      </c>
+      <c r="M76" t="s">
+        <v>163</v>
+      </c>
+      <c r="N76" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14">
+      <c r="A77">
+        <v>1</v>
+      </c>
+      <c r="B77">
+        <v>23</v>
+      </c>
+      <c r="C77" t="s">
+        <v>89</v>
+      </c>
+      <c r="D77">
+        <v>11</v>
+      </c>
+      <c r="E77" t="s">
+        <v>92</v>
+      </c>
+      <c r="F77">
+        <v>0.7</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77">
+        <v>0.62</v>
+      </c>
+      <c r="I77" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J77" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K77">
+        <v>30755967</v>
+      </c>
+      <c r="L77">
+        <v>900095597178</v>
+      </c>
+      <c r="M77" t="s">
+        <v>164</v>
+      </c>
+      <c r="N77" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14">
+      <c r="A78">
+        <v>1</v>
+      </c>
+      <c r="B78">
+        <v>29</v>
+      </c>
+      <c r="C78" t="s">
+        <v>90</v>
+      </c>
+      <c r="D78">
+        <v>12</v>
+      </c>
+      <c r="E78" t="s">
+        <v>92</v>
+      </c>
+      <c r="F78">
+        <v>0.7</v>
+      </c>
+      <c r="G78">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="H78">
+        <v>0.52</v>
+      </c>
+      <c r="I78" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J78" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K78">
+        <v>31967757</v>
+      </c>
+      <c r="L78">
+        <v>900095597294</v>
+      </c>
+      <c r="M78" t="s">
+        <v>165</v>
+      </c>
+      <c r="N78" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14">
+      <c r="A79">
+        <v>1</v>
+      </c>
+      <c r="B79">
+        <v>30</v>
+      </c>
+      <c r="C79" t="s">
+        <v>91</v>
+      </c>
+      <c r="D79">
+        <v>12</v>
+      </c>
+      <c r="E79" t="s">
+        <v>92</v>
+      </c>
+      <c r="F79">
+        <v>0.72</v>
+      </c>
+      <c r="G79">
+        <v>0.71</v>
+      </c>
+      <c r="H79">
+        <v>0.76</v>
+      </c>
+      <c r="I79" s="2">
+        <v>44960</v>
+      </c>
+      <c r="J79" s="2">
+        <v>45275</v>
+      </c>
+      <c r="K79">
+        <v>31264672</v>
+      </c>
+      <c r="L79">
+        <v>900095598212</v>
+      </c>
+      <c r="M79" t="s">
+        <v>166</v>
+      </c>
+      <c r="N79" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>